<commit_message>
Updated the aqi sensors dataset
</commit_message>
<xml_diff>
--- a/datasets/aqi_sensor_data.xlsx
+++ b/datasets/aqi_sensor_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robocop\PycharmProjects\bsa-assignment-saptarshi\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97697A9F-9F88-4217-A9DA-993E7BA0BC6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4AF146F-A309-46F6-A670-BF4BD32C5DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="58">
   <si>
     <t>name</t>
   </si>
@@ -115,6 +115,90 @@
   </si>
   <si>
     <t>Saturday, 03 Apr 2021 03:00 PM</t>
+  </si>
+  <si>
+    <t>Thursday, 01 Apr 2021 10:00 AM</t>
+  </si>
+  <si>
+    <t>Friday, 02 Apr 2021 10:00 AM</t>
+  </si>
+  <si>
+    <t>Saturday, 03 Apr 2021 10:00 AM</t>
+  </si>
+  <si>
+    <t>Sunday, 04 Apr 2021 10:00 AM</t>
+  </si>
+  <si>
+    <t>Monday, 05 Apr 2021 10:00 AM</t>
+  </si>
+  <si>
+    <t>Tuesday, 06 Apr 2021 10:00 AM</t>
+  </si>
+  <si>
+    <t>Wednesday, 07 Apr 2021 10:00 AM</t>
+  </si>
+  <si>
+    <t>Friday, 09 Apr 2021 10:00 AM</t>
+  </si>
+  <si>
+    <t>Saturday, 10 Apr 2021 10:00 AM</t>
+  </si>
+  <si>
+    <t>Sunday, 11 Apr 2021 10:00 AM</t>
+  </si>
+  <si>
+    <t>Monday, 12 Apr 2021 10:00 AM</t>
+  </si>
+  <si>
+    <t>Wednesday, 14 Apr 2021 10:00 AM</t>
+  </si>
+  <si>
+    <t>Thursday, 15 Apr 2021 10:00 AM</t>
+  </si>
+  <si>
+    <t>Friday, 16 Apr 2021 10:00 AM</t>
+  </si>
+  <si>
+    <t>Saturday, 17 Apr 2021 10:00 AM</t>
+  </si>
+  <si>
+    <t>Sunday, 18 Apr 2021 10:00 AM</t>
+  </si>
+  <si>
+    <t>Monday, 19 Apr 2021 10:00 AM</t>
+  </si>
+  <si>
+    <t>Tuesday, 20 Apr 2021 10:00 AM</t>
+  </si>
+  <si>
+    <t>Wednesday, 21 Apr 2021 10:00 AM</t>
+  </si>
+  <si>
+    <t>Thursday, 22 Apr 2021 10:00 AM</t>
+  </si>
+  <si>
+    <t>Friday, 23 Apr 2021 10:00 AM</t>
+  </si>
+  <si>
+    <t>Saturday, 24 Apr 2021 10:00 AM</t>
+  </si>
+  <si>
+    <t>Sunday, 25 Apr 2021 10:00 AM</t>
+  </si>
+  <si>
+    <t>Monday, 26 Apr 2021 10:00 AM</t>
+  </si>
+  <si>
+    <t>Tuesday, 27 Apr 2021 10:00 AM</t>
+  </si>
+  <si>
+    <t>Wednesday, 28 Apr 2021 10:00 AM</t>
+  </si>
+  <si>
+    <t>Thursday, 29 Apr 2021 10:00 AM</t>
+  </si>
+  <si>
+    <t>Friday, 30 Apr 2021 10:00 AM</t>
   </si>
 </sst>
 </file>
@@ -448,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -845,9 +929,312 @@
         <v>251</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" ht="15.75">
       <c r="A36" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.75">
+      <c r="A37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15.75">
+      <c r="A38" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15.75">
+      <c r="A39" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15.75">
+      <c r="A40" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C40">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15.75">
+      <c r="A41" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C41">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15.75">
+      <c r="A42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15.75">
+      <c r="A43" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.75">
+      <c r="A44" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15.75">
+      <c r="A45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C45">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15.75">
+      <c r="A46" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C46">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15.75">
+      <c r="A47" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C47">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15.75">
+      <c r="A48" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C48">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.75">
+      <c r="A49" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C49">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15.75">
+      <c r="A50" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C50">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15.75">
+      <c r="A51" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C51">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15.75">
+      <c r="A52" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C52">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15.75">
+      <c r="A53" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C53">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="15.75">
+      <c r="A54" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C54">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="15.75">
+      <c r="A55" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C55">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="15.75">
+      <c r="A56" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C56">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="15.75">
+      <c r="A57" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C57">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="15.75">
+      <c r="A58" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C58">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="15.75">
+      <c r="A59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C59">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="15.75">
+      <c r="A60" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C60">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="15.75">
+      <c r="A61" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C61">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="15.75">
+      <c r="A62" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C62">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="15.75">
+      <c r="A63" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C63">
+        <v>369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added raster analysis for aerosol levels data
</commit_message>
<xml_diff>
--- a/datasets/aqi_sensor_data.xlsx
+++ b/datasets/aqi_sensor_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robocop\PycharmProjects\bsa-assignment-saptarshi\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4AF146F-A309-46F6-A670-BF4BD32C5DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F3EEFB-E934-44FE-8847-E10155622C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -534,7 +534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added summary document and multiple timeline aerosol layers
</commit_message>
<xml_diff>
--- a/datasets/aqi_sensor_data.xlsx
+++ b/datasets/aqi_sensor_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robocop\PycharmProjects\bsa-assignment-saptarshi\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F3EEFB-E934-44FE-8847-E10155622C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692A2F1F-B559-47B6-99D6-0AC831836C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -534,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>